<commit_message>
Added cool design for user profile
</commit_message>
<xml_diff>
--- a/files/documentation/FrontendTimeline.xlsx
+++ b/files/documentation/FrontendTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7648CD93-1F36-4073-BD47-B5AE4AC5C950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F0451A-9114-4D78-9E32-4EC5DA740994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Day</t>
   </si>
@@ -43,10 +43,13 @@
     <t>Made login/signup page with some login functionality</t>
   </si>
   <si>
-    <t>30/3/2024</t>
-  </si>
-  <si>
     <t>Finished Login/SignUp/Forgot Password functionality in UI</t>
+  </si>
+  <si>
+    <t>30/4/2024</t>
+  </si>
+  <si>
+    <t>Added user profile functionality with cool starting design</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
   <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D10" sqref="D10:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -450,20 +453,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>3.25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45662</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" s="1"/>
@@ -479,7 +490,7 @@
       </c>
       <c r="D10" s="4">
         <f>SUM(C4:C9)</f>
-        <v>7.25</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
added user settings (just Ui), need to complete them
</commit_message>
<xml_diff>
--- a/files/documentation/FrontendTimeline.xlsx
+++ b/files/documentation/FrontendTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F0451A-9114-4D78-9E32-4EC5DA740994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F087219A-57D3-41DC-B9E3-EABE3B071D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
mostly finished user basic details update + change email + change password
</commit_message>
<xml_diff>
--- a/files/documentation/FrontendTimeline.xlsx
+++ b/files/documentation/FrontendTimeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F087219A-57D3-41DC-B9E3-EABE3B071D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE6311C-36C4-42DB-8C01-B7FF59D010D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31455" yWindow="-6060" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Day</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Added user profile functionality with cool starting design</t>
+  </si>
+  <si>
+    <t>Finished Mostly User Basic profile update, password reset, email change</t>
   </si>
 </sst>
 </file>
@@ -391,7 +394,7 @@
   <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -477,9 +480,18 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45874</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" s="3"/>
@@ -490,7 +502,7 @@
       </c>
       <c r="D10" s="4">
         <f>SUM(C4:C9)</f>
-        <v>11.75</v>
+        <v>16.75</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
Added categories in FE with design + Search Bar
</commit_message>
<xml_diff>
--- a/files/documentation/FrontendTimeline.xlsx
+++ b/files/documentation/FrontendTimeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD517809-F7D5-4A00-9C01-D045C6F4259B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BF3DB7-63E4-4D8D-8C6C-062505F73840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Day</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>Added Username reset and integrated with new phases functionality on BE</t>
+  </si>
+  <si>
+    <t>19/5/2024</t>
+  </si>
+  <si>
+    <t>Added categories in FE with design + Search Bar</t>
   </si>
 </sst>
 </file>
@@ -394,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -511,29 +517,43 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="B10" s="3"/>
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="4">
-        <f>SUM(C4:C9)</f>
-        <v>18.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4">
+        <f>SUM(C4:C10)</f>
+        <v>21.25</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
     </row>
+    <row r="14" spans="1:4">
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>